<commit_message>
mise à jour du journal
</commit_message>
<xml_diff>
--- a/assets/documents/133_GESTPROJ_G02.xlsx
+++ b/assets/documents/133_GESTPROJ_G02.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3ème année\Module 133\EMF-Shelf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\3ème année\Module 133\EMF-Shelf\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AA4899-EE31-4E33-AF9B-EDCEC1ACA552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BBE716-16FC-4122-85C1-E1C541FE4BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>Planning</t>
   </si>
@@ -888,6 +888,93 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -925,93 +1012,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1357,8 +1357,8 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1368,67 +1368,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="35"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
       <c r="O3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="33">
+      <c r="P3" s="62">
         <v>300233</v>
       </c>
-      <c r="Q3" s="35"/>
+      <c r="Q3" s="64"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="35"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="64"/>
       <c r="O4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1438,32 +1438,32 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="36" t="s">
+      <c r="C7" s="66"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="36" t="s">
+      <c r="F7" s="66"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="36" t="s">
+      <c r="L7" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="37"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="36" t="s">
+      <c r="M7" s="66"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="67"/>
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
@@ -1520,411 +1520,417 @@
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="29" t="s">
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="44"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="49"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="36"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="49"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="36"/>
     </row>
     <row r="11" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="42" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="49"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="36"/>
     </row>
     <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="51" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="49"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="36"/>
     </row>
     <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="52" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="44"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="49"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="36"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="49"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="36"/>
     </row>
     <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="49"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="36"/>
     </row>
     <row r="16" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="49"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="49"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="36"/>
     </row>
     <row r="18" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49" t="s">
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="H18" s="53"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="44"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="49"/>
+      <c r="H18" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="36"/>
     </row>
     <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="48" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="44"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="49"/>
+      <c r="H19" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="36"/>
     </row>
     <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="49"/>
+      <c r="H20" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="36"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="49"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="36"/>
     </row>
     <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="49"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="36"/>
     </row>
     <row r="23" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="53"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="49"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="36"/>
     </row>
     <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="66"/>
-      <c r="Q24" s="58"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="45"/>
     </row>
     <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="66"/>
-      <c r="Q25" s="67"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="54"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="64"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="64"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1958,7 +1964,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,11 +1975,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2039,9 +2045,15 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="16">
+        <v>45022</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="17">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -2100,7 +2112,7 @@
       <c r="B22" s="13"/>
       <c r="C22" s="17">
         <f>SUM(C8:C21)</f>
-        <v>7</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2154,7 +2166,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,11 +2177,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -2235,9 +2247,15 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="16">
+        <v>45022</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="17">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -2296,7 +2314,7 @@
       <c r="B22" s="13"/>
       <c r="C22" s="17">
         <f>SUM(C8:C21)</f>
-        <v>7</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2343,12 +2361,59 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2794,65 +2859,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
+    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2878,12 +2899,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>